<commit_message>
Update attendance report: Y2_B2526_Respiratory_session_analysis.xlsx
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_Respiratory_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_Respiratory_session_analysis.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Session Analysis Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,14 +58,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0090EE90"/>
-        <bgColor rgb="0090EE90"/>
+        <fgColor rgb="00FFB6C1"/>
+        <bgColor rgb="00FFB6C1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFB6C1"/>
-        <bgColor rgb="00FFB6C1"/>
+        <fgColor rgb="0090EE90"/>
+        <bgColor rgb="0090EE90"/>
       </patternFill>
     </fill>
   </fills>
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -93,19 +93,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -487,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="50" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -799,7 +796,7 @@
         </is>
       </c>
       <c r="L6" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -850,7 +847,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -953,7 +950,7 @@
       </c>
       <c r="L9" s="4" t="inlineStr">
         <is>
-          <t>2.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1003,7 @@
       </c>
       <c r="L10" s="4" t="inlineStr">
         <is>
-          <t>12.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1447,22 +1444,22 @@
         <v>16</v>
       </c>
       <c r="O17" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="P17" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="Q17" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
-          <t>6.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S17" s="4" t="inlineStr">
         <is>
-          <t>0.9%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1525,22 +1522,22 @@
         <v>16</v>
       </c>
       <c r="O18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="P18" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="Q18" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R18" s="4" t="inlineStr">
         <is>
-          <t>6.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S18" s="4" t="inlineStr">
         <is>
-          <t>35.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -1681,22 +1678,22 @@
         <v>16</v>
       </c>
       <c r="O20" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="4" t="n">
         <v>1</v>
-      </c>
-      <c r="P20" s="4" t="n">
-        <v>0</v>
       </c>
       <c r="Q20" s="4" t="n">
         <v>15</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
-          <t>6.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="S20" s="4" t="inlineStr">
         <is>
-          <t>0.4%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -2425,19 +2422,15 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G34" s="8" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, nahla.nagiub@med.asu.edu.eg, rana.abozaid@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G34" s="8" t="inlineStr"/>
       <c r="H34" s="8" t="inlineStr">
         <is>
-          <t>2/220</t>
+          <t>0/220</t>
         </is>
       </c>
       <c r="I34" s="8" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -3117,19 +3110,15 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G50" s="8" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, nahla.nagiub@med.asu.edu.eg, rana.abozaid@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G50" s="8" t="inlineStr"/>
       <c r="H50" s="8" t="inlineStr">
         <is>
-          <t>79/225</t>
+          <t>0/225</t>
         </is>
       </c>
       <c r="I50" s="8" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>
@@ -3779,43 +3768,43 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="9" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B66" s="9" t="inlineStr">
+      <c r="A66" s="8" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B66" s="8" t="inlineStr">
         <is>
           <t>B1</t>
         </is>
       </c>
-      <c r="C66" s="9" t="inlineStr">
+      <c r="C66" s="8" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D66" s="9" t="inlineStr">
+      <c r="D66" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E66" s="9" t="inlineStr">
+      <c r="E66" s="8" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="F66" s="9" t="inlineStr">
+      <c r="F66" s="8" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G66" s="9" t="inlineStr"/>
-      <c r="H66" s="9" t="inlineStr">
+      <c r="G66" s="8" t="inlineStr"/>
+      <c r="H66" s="8" t="inlineStr">
         <is>
           <t>0/154</t>
         </is>
       </c>
-      <c r="I66" s="9" t="inlineStr">
+      <c r="I66" s="8" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -4497,19 +4486,15 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G82" s="8" t="inlineStr">
-        <is>
-          <t>mennatulla.medhat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, nahla.nagiub@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
-        </is>
-      </c>
+      <c r="G82" s="8" t="inlineStr"/>
       <c r="H82" s="8" t="inlineStr">
         <is>
-          <t>1/224</t>
+          <t>0/224</t>
         </is>
       </c>
       <c r="I82" s="8" t="inlineStr">
         <is>
-          <t>Recorded</t>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Daily attendance processing - 2026-02-08 09:46:04 UTC
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_Respiratory_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_Respiratory_session_analysis.xlsx
@@ -484,7 +484,7 @@
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
+    <col width="31" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
     <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
@@ -1038,7 +1038,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G11" s="2" t="inlineStr"/>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
           <t>153/216</t>
@@ -1081,7 +1085,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr"/>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H12" s="2" t="inlineStr">
         <is>
           <t>153/216</t>
@@ -2076,7 +2084,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G27" s="2" t="inlineStr"/>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
           <t>183/217</t>
@@ -2134,7 +2146,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr"/>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
           <t>183/217</t>
@@ -2809,7 +2825,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G43" s="2" t="inlineStr"/>
+      <c r="G43" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
           <t>205/220</t>
@@ -2852,7 +2872,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G44" s="2" t="inlineStr"/>
+      <c r="G44" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
           <t>205/220</t>
@@ -3497,7 +3521,11 @@
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G59" s="2" t="inlineStr"/>
+      <c r="G59" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
           <t>161/225</t>
@@ -3540,7 +3568,11 @@
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G60" s="2" t="inlineStr"/>
+      <c r="G60" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
           <t>161/225</t>
@@ -4185,7 +4217,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G75" s="2" t="inlineStr"/>
+      <c r="G75" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H75" s="2" t="inlineStr">
         <is>
           <t>141/154</t>
@@ -4228,7 +4264,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G76" s="2" t="inlineStr"/>
+      <c r="G76" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H76" s="2" t="inlineStr">
         <is>
           <t>141/154</t>
@@ -4873,7 +4913,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G91" s="2" t="inlineStr"/>
+      <c r="G91" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H91" s="2" t="inlineStr">
         <is>
           <t>203/224</t>
@@ -4916,7 +4960,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G92" s="2" t="inlineStr"/>
+      <c r="G92" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
           <t>203/224</t>
@@ -5561,7 +5609,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G107" s="2" t="inlineStr"/>
+      <c r="G107" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H107" s="2" t="inlineStr">
         <is>
           <t>136/224</t>
@@ -5604,7 +5656,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G108" s="2" t="inlineStr"/>
+      <c r="G108" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H108" s="2" t="inlineStr">
         <is>
           <t>136/224</t>
@@ -6249,7 +6305,11 @@
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G123" s="2" t="inlineStr"/>
+      <c r="G123" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H123" s="2" t="inlineStr">
         <is>
           <t>124/226</t>
@@ -6292,7 +6352,11 @@
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G124" s="2" t="inlineStr"/>
+      <c r="G124" s="2" t="inlineStr">
+        <is>
+          <t>mona.I.hussein@med.asu.edu.eg</t>
+        </is>
+      </c>
       <c r="H124" s="2" t="inlineStr">
         <is>
           <t>124/226</t>

</xml_diff>